<commit_message>
Added table creation functions for lehrer, noten, schueler(not done yet)
</commit_message>
<xml_diff>
--- a/planing/resoruces/database blueprints/lehrer.xlsx
+++ b/planing/resoruces/database blueprints/lehrer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fabian\Documents\NOTENRECHNER\final\planing\resoruces\database blueprints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4843C201-D64E-4111-BEC1-EA631A76B852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B563D82E-A92C-40A6-8A38-9DDD01B8FFE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Lehrer_kürzel</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>kommentar</t>
+  </si>
+  <si>
+    <t>Lehrer_ID</t>
   </si>
 </sst>
 </file>
@@ -384,64 +387,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" customWidth="1"/>
-    <col min="4" max="4" width="21.21875" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" customWidth="1"/>
-    <col min="14" max="14" width="14.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.77734375" customWidth="1"/>
+    <col min="5" max="5" width="21.21875" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="16.88671875" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" customWidth="1"/>
+    <col min="15" max="15" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>